<commit_message>
Avance de memoria y proyecto
Se realiza cambio de diseño de interfaz, tanto en el login, tabla de búsqueda de eventos,  parte de las vistas de solicitud y en ingresar resolución. Ademas, está el generar pdf incompleto junto con categorías e ingresar personas en la etapa de solicitud.

Por otro lado, se encuentran las correcciones de la ultima reunión del profe guía antes de terminar el semestre.
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B2D393-A135-42E6-9A61-441123F24185}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A89A0AE-258D-46FF-8A95-E992E44DD6F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planificación principal" sheetId="3" r:id="rId1"/>
+    <sheet name="Planificación modificada" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -18,6 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Número</t>
   </si>
@@ -133,13 +135,37 @@
   </si>
   <si>
     <t>Semanas</t>
+  </si>
+  <si>
+    <t>Pruebas de usabilidad</t>
+  </si>
+  <si>
+    <t>Modificar documentación de memoria</t>
+  </si>
+  <si>
+    <t>Subir una copia del documento de resolución</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Solicitud y  Resolución </t>
+  </si>
+  <si>
+    <t>Aceptar Solicitud y agregar Resolución</t>
+  </si>
+  <si>
+    <t>4. Rendición</t>
+  </si>
+  <si>
+    <t>5. Usuario</t>
+  </si>
+  <si>
+    <t>6. Documentación y Panel de Ayuda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +173,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,8 +201,116 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -191,11 +333,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,31 +468,165 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,11 +907,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0725F9CB-67EE-4779-A6EA-F76A6A4E8FF0}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,34 +925,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
     </row>
     <row r="2" spans="1:30" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -571,87 +967,87 @@
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>3</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>4</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="2">
         <v>5</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="2">
         <v>6</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="2">
         <v>7</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <v>8</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2">
         <v>9</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="2">
         <v>10</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="2">
         <v>11</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="2">
         <v>12</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="2">
         <v>13</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="2">
         <v>14</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="2">
         <v>15</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T2" s="2">
         <v>16</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="2">
         <v>17</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="2">
         <v>18</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="2">
         <v>19</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="2">
         <v>20</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="2">
         <v>21</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="2">
         <v>22</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="2">
         <v>23</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="2">
         <v>24</v>
       </c>
-      <c r="AC2" s="8">
+      <c r="AC2" s="2">
         <v>25</v>
       </c>
-      <c r="AD2" s="8">
+      <c r="AD2" s="2">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -659,8 +1055,8 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -683,11 +1079,11 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
     </row>
     <row r="4" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -695,7 +1091,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -717,11 +1113,11 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
     </row>
     <row r="5" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
@@ -729,8 +1125,8 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -751,11 +1147,11 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
     </row>
     <row r="6" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -767,7 +1163,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -787,11 +1183,11 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -802,7 +1198,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="5"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -821,11 +1217,11 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
@@ -836,8 +1232,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -855,11 +1251,11 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -870,7 +1266,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -889,8 +1285,8 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
     </row>
     <row r="10" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -907,10 +1303,10 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -925,11 +1321,11 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -947,7 +1343,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="5"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -961,11 +1357,11 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
@@ -982,8 +1378,8 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
@@ -995,11 +1391,11 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1017,9 +1413,9 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
@@ -1029,11 +1425,11 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1056,7 +1452,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-      <c r="T14" s="5"/>
+      <c r="T14" s="4"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -1065,11 +1461,11 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
     </row>
     <row r="15" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1487,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
-      <c r="U15" s="5"/>
+      <c r="U15" s="4"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
@@ -1099,11 +1495,11 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
     </row>
     <row r="16" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
@@ -1125,7 +1521,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
-      <c r="U16" s="5"/>
+      <c r="U16" s="4"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
@@ -1133,11 +1529,11 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
     </row>
     <row r="17" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1160,18 +1556,18 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="5"/>
+      <c r="V17" s="4"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1195,17 +1591,17 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="5"/>
+      <c r="W18" s="4"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
     </row>
     <row r="19" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="32" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1232,16 +1628,16 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-      <c r="X19" s="5"/>
+      <c r="X19" s="4"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
     </row>
     <row r="20" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1266,16 +1662,16 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-      <c r="X20" s="5"/>
+      <c r="X20" s="4"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
     </row>
     <row r="21" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
@@ -1300,16 +1696,16 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="6"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1335,15 +1731,15 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="6"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
     </row>
     <row r="23" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1370,14 +1766,14 @@
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
-      <c r="Z23" s="7"/>
+      <c r="Z23" s="5"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
     </row>
     <row r="24" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="32" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1407,13 +1803,13 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
-      <c r="AA24" s="7"/>
+      <c r="AA24" s="5"/>
       <c r="AB24" s="2"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
     </row>
     <row r="25" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
@@ -1442,12 +1838,12 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
-      <c r="AB25" s="7"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
     </row>
     <row r="26" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1477,19 +1873,1137 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
-      <c r="AC26" s="10"/>
-      <c r="AD26" s="10"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A19:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="E1:AD1"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5546875" style="1" customWidth="1"/>
+    <col min="14" max="15" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="25" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+    </row>
+    <row r="2" spans="1:25" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="56">
+        <v>1</v>
+      </c>
+      <c r="D2" s="56">
+        <v>2</v>
+      </c>
+      <c r="E2" s="56">
+        <v>3</v>
+      </c>
+      <c r="F2" s="56">
+        <v>4</v>
+      </c>
+      <c r="G2" s="56">
+        <v>5</v>
+      </c>
+      <c r="H2" s="56">
+        <v>6</v>
+      </c>
+      <c r="I2" s="56">
+        <v>7</v>
+      </c>
+      <c r="J2" s="56">
+        <v>8</v>
+      </c>
+      <c r="K2" s="56">
+        <v>9</v>
+      </c>
+      <c r="L2" s="56">
+        <v>10</v>
+      </c>
+      <c r="M2" s="56">
+        <v>11</v>
+      </c>
+      <c r="N2" s="56">
+        <v>12</v>
+      </c>
+      <c r="O2" s="56">
+        <v>13</v>
+      </c>
+      <c r="P2" s="56">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="56">
+        <v>15</v>
+      </c>
+      <c r="R2" s="56">
+        <v>16</v>
+      </c>
+      <c r="S2" s="56">
+        <v>17</v>
+      </c>
+      <c r="T2" s="56">
+        <v>18</v>
+      </c>
+      <c r="U2" s="56">
+        <v>19</v>
+      </c>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+    </row>
+    <row r="3" spans="1:25" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57">
+        <v>43556</v>
+      </c>
+      <c r="K3" s="57">
+        <f>SUM(J3,7)</f>
+        <v>43563</v>
+      </c>
+      <c r="L3" s="57">
+        <f t="shared" ref="L3:U3" si="0">SUM(K3,7)</f>
+        <v>43570</v>
+      </c>
+      <c r="M3" s="57">
+        <f t="shared" si="0"/>
+        <v>43577</v>
+      </c>
+      <c r="N3" s="57">
+        <f t="shared" si="0"/>
+        <v>43584</v>
+      </c>
+      <c r="O3" s="57">
+        <f t="shared" si="0"/>
+        <v>43591</v>
+      </c>
+      <c r="P3" s="57">
+        <f t="shared" si="0"/>
+        <v>43598</v>
+      </c>
+      <c r="Q3" s="57">
+        <f t="shared" si="0"/>
+        <v>43605</v>
+      </c>
+      <c r="R3" s="57">
+        <f t="shared" si="0"/>
+        <v>43612</v>
+      </c>
+      <c r="S3" s="57">
+        <f t="shared" si="0"/>
+        <v>43619</v>
+      </c>
+      <c r="T3" s="57">
+        <f t="shared" si="0"/>
+        <v>43626</v>
+      </c>
+      <c r="U3" s="57">
+        <f t="shared" si="0"/>
+        <v>43633</v>
+      </c>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+    </row>
+    <row r="4" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="52">
+        <v>100</v>
+      </c>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="30">
+        <v>100</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="35"/>
+      <c r="B6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="46">
+        <v>100</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+    </row>
+    <row r="7" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="31">
+        <v>80</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="37"/>
+      <c r="B8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="31">
+        <v>70</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="37"/>
+      <c r="B9" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="31">
+        <v>70</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+    </row>
+    <row r="10" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="30">
+        <v>100</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+    </row>
+    <row r="11" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+    </row>
+    <row r="12" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="39"/>
+      <c r="B12" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="39"/>
+      <c r="B13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="39"/>
+      <c r="B14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="39"/>
+      <c r="B15" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="39"/>
+      <c r="B16" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="39"/>
+      <c r="B17" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+    </row>
+    <row r="18" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="39"/>
+      <c r="B18" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="39"/>
+      <c r="B19" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A20" s="39"/>
+      <c r="B20" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="42"/>
+      <c r="B23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="42"/>
+      <c r="B24" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="29">
+        <v>100</v>
+      </c>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" s="42"/>
+      <c r="B25" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="14"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="45"/>
+      <c r="B27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="14"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="45"/>
+      <c r="B28" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="14"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" s="45"/>
+      <c r="B29" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="14"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" s="45"/>
+      <c r="B30" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="14"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" s="43"/>
+      <c r="B32" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A33" s="43"/>
+      <c r="B33" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="16"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C1:U1"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A21"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A26:A30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>